<commit_message>
Improved pin map file.
</commit_message>
<xml_diff>
--- a/Documentation/uc to mpide pin converter for default64.xlsx
+++ b/Documentation/uc to mpide pin converter for default64.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\mpide_STP300\Documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA63B62-A4F6-41AC-949C-9246B5D095E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>in</t>
   </si>
@@ -31,14 +48,151 @@
   </si>
   <si>
     <t>d11</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>cK Pin</t>
+  </si>
+  <si>
+    <t>uC Pin</t>
+  </si>
+  <si>
+    <t>JP0-ID+1</t>
+  </si>
+  <si>
+    <t>JP1-ID+2</t>
+  </si>
+  <si>
+    <t>JP2-ID+3</t>
+  </si>
+  <si>
+    <t>uC Reg</t>
+  </si>
+  <si>
+    <t>RC13</t>
+  </si>
+  <si>
+    <t>RC14</t>
+  </si>
+  <si>
+    <t>RD0</t>
+  </si>
+  <si>
+    <t>PROG1</t>
+  </si>
+  <si>
+    <t>PROG2</t>
+  </si>
+  <si>
+    <t>DEBUG_LED</t>
+  </si>
+  <si>
+    <t>RD4</t>
+  </si>
+  <si>
+    <t>RD5</t>
+  </si>
+  <si>
+    <t>RF0</t>
+  </si>
+  <si>
+    <t>LED0</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>RE2</t>
+  </si>
+  <si>
+    <t>RE3</t>
+  </si>
+  <si>
+    <t>485_ENABLE</t>
+  </si>
+  <si>
+    <t>RE4</t>
+  </si>
+  <si>
+    <t>Signal/Var</t>
+  </si>
+  <si>
+    <t>HOME1</t>
+  </si>
+  <si>
+    <t>HOME2</t>
+  </si>
+  <si>
+    <t>RE5</t>
+  </si>
+  <si>
+    <t>RE6</t>
+  </si>
+  <si>
+    <t>BUSY</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>FLAG</t>
+  </si>
+  <si>
+    <t>STEP_INPUT</t>
+  </si>
+  <si>
+    <t>RB3</t>
+  </si>
+  <si>
+    <t>RB2</t>
+  </si>
+  <si>
+    <t>RB1</t>
+  </si>
+  <si>
+    <t>RB0</t>
+  </si>
+  <si>
+    <t>RELAY1</t>
+  </si>
+  <si>
+    <t>RELAY2</t>
+  </si>
+  <si>
+    <t>TCK</t>
+  </si>
+  <si>
+    <t>TDI</t>
+  </si>
+  <si>
+    <t>RD1</t>
+  </si>
+  <si>
+    <t>RD2</t>
+  </si>
+  <si>
+    <t>485-U1RX</t>
+  </si>
+  <si>
+    <t>485-U1TX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -72,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -80,12 +234,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -132,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -164,9 +327,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,6 +379,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -373,71 +572,309 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="I1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>46</v>
+      </c>
+      <c r="C2">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <f>(CODE(B2)-CODE("a"))*16+MID(B2,2,10)</f>
+      <c r="I2" s="1">
+        <f>(CODE(H2)-CODE("a"))*16+MID(H2,2,10)</f>
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2">
+      <c r="H3" s="2">
         <v>68</v>
       </c>
-      <c r="C3" s="1" t="str">
-        <f>CHAR((B3-(MOD(B3,16)))/16+CODE("a"))&amp;MOD(B3,16)</f>
+      <c r="I3" s="1" t="str">
+        <f>CHAR((H3-(MOD(H3,16)))/16+CODE("a"))&amp;MOD(H3,16)</f>
         <v>e4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>48</v>
+      </c>
+      <c r="C4">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>62</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20">
+        <v>28</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24">
+        <v>51</v>
+      </c>
+      <c r="D24" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>